<commit_message>
work on captcha requirement
</commit_message>
<xml_diff>
--- a/docs/容量规划.xlsx
+++ b/docs/容量规划.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1100" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="4120" yWindow="1320" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>单个对象大小</t>
     <rPh sb="0" eb="1">
@@ -113,6 +113,114 @@
     <rPh sb="5" eb="6">
       <t>ck</t>
     </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集层</t>
+    <rPh sb="0" eb="1">
+      <t>eswy</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>nfc</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成器</t>
+    <rPh sb="0" eb="1">
+      <t>tgd</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>kkd</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载器</t>
+    <rPh sb="0" eb="1">
+      <t>gh</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>fa</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>kkd</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结构化层</t>
+    <rPh sb="0" eb="1">
+      <t>xfs</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>wx</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>nfc</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存储层</t>
+    <rPh sb="0" eb="1">
+      <t>dhw</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>nfc</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解析器</t>
+    <rPh sb="0" eb="1">
+      <t>qes</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>kkd</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MySQL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MongoDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+    <rPh sb="0" eb="1">
+      <t>ovj</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置</t>
+    <rPh sb="0" eb="1">
+      <t>sgl</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disk 2T * CPU 8 * Mem 32G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disk 300G * CPU 8 * Mem 32G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disk 300G * CPU 8 * Mem 32G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disk 300G * CPU 8 * Mem 32G</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -436,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G7"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,7 +555,7 @@
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -521,6 +629,95 @@
         <v>3.8580246913580241</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>